<commit_message>
atualiza post das leituras
</commit_message>
<xml_diff>
--- a/posts/2024-07-25-leituras-1sem/pt/dados/tabela_leituras.xlsx
+++ b/posts/2024-07-25-leituras-1sem/pt/dados/tabela_leituras.xlsx
@@ -355,13 +355,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="18" max="18" width="20.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
@@ -382,59 +382,59 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>mes_leitura_inicio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>mes_leitura_fim</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ordem</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>nome</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>ano_publicacao_original</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>editora</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>n_paginas</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>idioma_leitura</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>tipo</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>genero</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>autoria_nome</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>autoria_genero</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>autoria_raca</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>autoria_pais</t>
-        </is>
-      </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
           <t>extra_tags</t>
@@ -442,20 +442,25 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>url_capa</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>nota_skoob</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>n_avaliacoes_skoob</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>atualizacao_nota_skoob</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>link_skoob</t>
         </is>
@@ -475,65 +480,68 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Janeiro</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Janeiro</t>
+        </is>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>Lifelong Leaners - O poder do aprendizado contínuo</t>
         </is>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>2021</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Gente</t>
         </is>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>256</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>físico</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Desenvolvimento Profissional</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>Conrado Schlochauer</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
-      <c r="P2">
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/vQumTIZjoHW7aOpwb78jexcI8mQ=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/11932482/LIFELONG_LEARNERS_162378052211932482SK-V11623780524B.jpg</t>
+        </is>
+      </c>
+      <c r="Q2">
         <v>4.2</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>197</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>45498</v>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/lifelong-learners-11932482ed11927229.html</t>
         </is>
@@ -553,65 +561,68 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>Janeiro</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Fevereiro</t>
+        </is>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>O andar do bêbado - Como o acaso determina nossas vidas</t>
         </is>
       </c>
-      <c r="E3">
+      <c r="H3">
         <v>2009</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Zahar</t>
         </is>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>264</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>ebook</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Divulgação científica</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>Leonard Mlodinow</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Estados Unidos</t>
-        </is>
-      </c>
-      <c r="P3">
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/Izg4EFJay00USCjkxO-7a-9vU2U=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/37134/O_ANDAR_DO_BEBADO_142236016637134SK1422360166B.jpg</t>
+        </is>
+      </c>
+      <c r="Q3">
         <v>4.1</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>3363</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>45498</v>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/o-andar-do-bebado-37134ed40631.html</t>
         </is>
@@ -631,65 +642,68 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Fevereiro</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Fevereiro</t>
+        </is>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>Como se faz uma tese</t>
         </is>
       </c>
-      <c r="E4">
+      <c r="H4">
         <v>1977</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Perspectiva</t>
         </is>
       </c>
-      <c r="G4">
+      <c r="J4">
         <v>224</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>físico</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>?</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>Umberto Eco</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Itália</t>
-        </is>
-      </c>
-      <c r="P4">
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/D8rKGijUhZsvy8Jm6S8Xao_bA60=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/1087887/COMO_SE_FAZ_UMA_TESE_15798907591087887SK1579890760B.jpg</t>
+        </is>
+      </c>
+      <c r="Q4">
         <v>4.2</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>49</v>
       </c>
-      <c r="R4" s="2">
+      <c r="S4" s="2">
         <v>45498</v>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/como-se-faz-uma-tese-1087887ed1090808.html</t>
         </is>
@@ -709,65 +723,68 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Março</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Março</t>
+        </is>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>A vida não é útil</t>
         </is>
       </c>
-      <c r="E5">
+      <c r="H5">
         <v>2020</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Companhia das Letras</t>
         </is>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>128</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>físico</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>Ciências sociais</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>Ailton Krenak</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>indígena</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
-      <c r="P5">
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/KAqRRckXv8IY8Xij99m7NTRffPg=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/1268557/A_VIDA_NAO_E_UTIL_15956282211268557SK1595628222B.jpg</t>
+        </is>
+      </c>
+      <c r="Q5">
         <v>4.4</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>3833</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <v>45498</v>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/a-vida-nao-e-util-1268557ed11627332.html</t>
         </is>
@@ -787,65 +804,68 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>Março</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Março</t>
+        </is>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>Duna</t>
         </is>
       </c>
-      <c r="E6">
+      <c r="H6">
         <v>1965</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Aleph</t>
         </is>
       </c>
-      <c r="G6">
+      <c r="J6">
         <v>680</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>ebook</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>Ficção científica</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>Frank Herbert</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Estados Unidos</t>
-        </is>
-      </c>
-      <c r="P6">
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/ggHUmbF0GSS7-VJC4BFCYE1ULqs=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/2278/DUNA_14922665702278SK1492266571B.jpg</t>
+        </is>
+      </c>
+      <c r="Q6">
         <v>4.5</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>21847</v>
       </c>
-      <c r="R6" s="2">
+      <c r="S6" s="2">
         <v>45498</v>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/duna-2278ed673523.html</t>
         </is>
@@ -865,65 +885,68 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>Março</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Abril</t>
+        </is>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>Messias de Duna</t>
         </is>
       </c>
-      <c r="E7">
+      <c r="H7">
         <v>1969</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Aleph</t>
         </is>
       </c>
-      <c r="G7">
+      <c r="J7">
         <v>272</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>ebook</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>Ficção científica</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>Frank Herbert</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>Estados Unidos</t>
-        </is>
-      </c>
-      <c r="P7">
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/apU0KFKa8MMC8_RC0Ow_nrLy-mg=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/689543/MESSIAS_DE_DUNA_1498133840689543SK1498133840B.jpg</t>
+        </is>
+      </c>
+      <c r="Q7">
         <v>4.1</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>240</v>
       </c>
-      <c r="R7" s="2">
+      <c r="S7" s="2">
         <v>45498</v>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="T7" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/messias-de-duna-689543ed692362.html</t>
         </is>
@@ -943,65 +966,68 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>Abril</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Abril</t>
+        </is>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>Filhos de Duna</t>
         </is>
       </c>
-      <c r="E8">
+      <c r="H8">
         <v>1976</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Aleph</t>
         </is>
       </c>
-      <c r="G8">
+      <c r="J8">
         <v>528</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>ebook</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>Ficção científica</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>Frank Herbert</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>Estados Unidos</t>
-        </is>
-      </c>
-      <c r="P8">
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/_TQPBBz05NWGGwdUNq6inCvng3M=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/1149196/09c3ad9a30ec24cf042d67f2ef2974e5B.jpg</t>
+        </is>
+      </c>
+      <c r="Q8">
         <v>4.1</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>59</v>
       </c>
-      <c r="R8" s="2">
+      <c r="S8" s="2">
         <v>45498</v>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/filhos-de-duna-cronicas-de-duna-livro-3-1149196ed1151450.html</t>
         </is>
@@ -1021,65 +1047,68 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>Abril</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>Imperador Deus de Duna</t>
         </is>
       </c>
-      <c r="E9">
+      <c r="H9">
         <v>1981</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Aleph</t>
         </is>
       </c>
-      <c r="G9">
+      <c r="J9">
         <v>512</v>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>ebook</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>Ficção científica</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>Frank Herbert</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>Estados Unidos</t>
-        </is>
-      </c>
-      <c r="P9">
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/UnhsMzn6WGcvQEAkf8WLl0q7uTA=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/6727/IMPERADOR_DEUS_DE_DUNA_16678365316727SK-V11667836533B.jpg</t>
+        </is>
+      </c>
+      <c r="Q9">
         <v>4.1</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>1515</v>
       </c>
-      <c r="R9" s="2">
+      <c r="S9" s="2">
         <v>45498</v>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/imperador-deus-de-duna-6727ed122233701.html</t>
         </is>
@@ -1099,65 +1128,68 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>Hereges de Duna</t>
         </is>
       </c>
-      <c r="E10">
+      <c r="H10">
         <v>1984</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Aleph</t>
         </is>
       </c>
-      <c r="G10">
+      <c r="J10">
         <v>568</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>ebook</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>Ficção científica</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>Frank Herbert</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>Estados Unidos</t>
-        </is>
-      </c>
-      <c r="P10">
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/JOaQUnYshQra3o9rl7FVNCR6npk=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/6429/HEREGES_DE_DUNA_15308262596429SK1530826259B.jpg</t>
+        </is>
+      </c>
+      <c r="Q10">
         <v>4.1</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>1008</v>
       </c>
-      <c r="R10" s="2">
+      <c r="S10" s="2">
         <v>45498</v>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="T10" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/hereges-de-duna-6429ed760647.html</t>
         </is>
@@ -1177,65 +1209,68 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>Herdeiras de Duna</t>
         </is>
       </c>
-      <c r="E11">
+      <c r="H11">
         <v>1985</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Aleph</t>
         </is>
       </c>
-      <c r="G11">
+      <c r="J11">
         <v>528</v>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>ebook</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>Ficção científica</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>Frank Herbert</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>Estados Unidos</t>
-        </is>
-      </c>
-      <c r="P11">
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/zXtX3Rl0F_iqnsYDs4nDYDKwH7E=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/6729/HERDEIRAS_DE_DUNA_16355961276729SK-V11635596128B.jpg</t>
+        </is>
+      </c>
+      <c r="Q11">
         <v>4</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>708</v>
       </c>
-      <c r="R11" s="2">
+      <c r="S11" s="2">
         <v>45498</v>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/herdeiras-de-duna-6729ed11676237.html</t>
         </is>
@@ -1255,70 +1290,73 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>Março</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Abril</t>
+        </is>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>Nós matamos o cão tinhoso!</t>
         </is>
       </c>
-      <c r="E12">
+      <c r="H12">
         <v>1964</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Kapulana</t>
         </is>
       </c>
-      <c r="G12">
+      <c r="J12">
         <v>148</v>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>físico</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>Contos</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>Luís Bernardo Honwana</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>negra</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>Moçambique</t>
-        </is>
-      </c>
       <c r="O12" t="inlineStr">
         <is>
           <t>vestibular</t>
         </is>
       </c>
-      <c r="P12">
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/U06I5lueQ-RDLsAsqc3a0nW_uu0=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/228379/NOS_MATAMOS_O_CAO_TINHOSO_1533409735228379SK1533409735B.jpg</t>
+        </is>
+      </c>
+      <c r="Q12">
         <v>3.8</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>1710</v>
       </c>
-      <c r="R12" s="2">
+      <c r="S12" s="2">
         <v>45498</v>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/nos-matamos-o-cao-tinhoso-228379ed734247.html</t>
         </is>
@@ -1338,70 +1376,73 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Junho</t>
+        </is>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>Primeiro Sangue</t>
         </is>
       </c>
-      <c r="E13">
+      <c r="H13">
         <v>2021</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>Europa Editions</t>
         </is>
       </c>
-      <c r="G13">
+      <c r="J13">
         <v>112</v>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>inglês</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>ebook</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>Ficção contemporânea</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>Amélie Nothomb</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>feminino</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>Bélgica</t>
-        </is>
-      </c>
       <c r="O13" t="inlineStr">
         <is>
           <t>TAG; TAG Curadoria</t>
         </is>
       </c>
-      <c r="P13">
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/9wSqfn96T99lQABFqs8NiKQpQUk=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/122443210/PRIMEIRO_SANGUE_1713758497122443210SK-V11713758498B.jpg</t>
+        </is>
+      </c>
+      <c r="Q13">
         <v>4</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>376</v>
       </c>
-      <c r="R13" s="2">
+      <c r="S13" s="2">
         <v>45498</v>
       </c>
-      <c r="S13" t="inlineStr">
+      <c r="T13" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/primeiro-sangue-122443210ed122448495.html</t>
         </is>
@@ -1421,70 +1462,73 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>Junho</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Junho</t>
+        </is>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>23 minutos</t>
         </is>
       </c>
-      <c r="E14">
-        <v>2024</v>
-      </c>
-      <c r="F14" t="inlineStr">
+      <c r="H14">
+        <v>2024</v>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>Harper Collins</t>
         </is>
       </c>
-      <c r="G14">
+      <c r="J14">
         <v>224</v>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>físico</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>Suspense; Mistério</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>Waldson Souza</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>negra</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
       <c r="O14" t="inlineStr">
         <is>
           <t>TAG; TAG Inéditos</t>
         </is>
       </c>
-      <c r="P14">
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/XXDOGJsrON-8_iaVeil9AwWH6Jg=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/122396276/23_MINUTOS_1716218901122396276SK-V11716218902B.jpg</t>
+        </is>
+      </c>
+      <c r="Q14">
         <v>3.8</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>504</v>
       </c>
-      <c r="R14" s="2">
+      <c r="S14" s="2">
         <v>45498</v>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="T14" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/23-minutos-122396276ed122397526.html</t>
         </is>
@@ -1504,70 +1548,73 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Junho</t>
+        </is>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Quincas Borba</t>
         </is>
       </c>
-      <c r="E15">
+      <c r="H15">
         <v>1891</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>Principis</t>
         </is>
       </c>
-      <c r="G15">
+      <c r="J15">
         <v>240</v>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>físico</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>Literatura; Ficção</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>Machado de Assis</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>negra</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
       <c r="O15" t="inlineStr">
         <is>
           <t>vestibular</t>
         </is>
       </c>
-      <c r="P15">
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/ti-sexCgLAnJw2fZdRmGEQ8UmGk=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/1010316/a5e5d070460bdaeab8b9b4ba7822baf5B.jpg</t>
+        </is>
+      </c>
+      <c r="Q15">
         <v>3.8</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>2406</v>
       </c>
-      <c r="R15" s="2">
+      <c r="S15" s="2">
         <v>45498</v>
       </c>
-      <c r="S15" t="inlineStr">
+      <c r="T15" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/quincas-borba-1010316ed1012277.html</t>
         </is>
@@ -1587,70 +1634,73 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>Junho</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>Dom Casmurro</t>
         </is>
       </c>
-      <c r="E16">
+      <c r="H16">
         <v>1899</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>Martin Claret</t>
         </is>
       </c>
-      <c r="G16">
+      <c r="J16">
         <v>408</v>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>físico</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>Literatura; Ficção</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>Machado de Assis</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>negra</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
       <c r="O16" t="inlineStr">
         <is>
           <t>vestibular</t>
         </is>
       </c>
-      <c r="P16">
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/4fidKiSyyErixh8I_E77QYP_NY0=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/180/DOM_CASMURRO_1627233540180SK-V11627233595B.jpg</t>
+        </is>
+      </c>
+      <c r="Q16">
         <v>4.2</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>108695</v>
       </c>
-      <c r="R16" s="2">
+      <c r="S16" s="2">
         <v>45498</v>
       </c>
-      <c r="S16" t="inlineStr">
+      <c r="T16" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/dom-casmurro-180ed11923771.html</t>
         </is>
@@ -1670,58 +1720,75 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>Junho</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>Os vulneráveis</t>
         </is>
       </c>
-      <c r="E17">
-        <v>2024</v>
-      </c>
-      <c r="F17" t="inlineStr">
+      <c r="H17">
+        <v>2024</v>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>Instante</t>
         </is>
       </c>
-      <c r="G17">
+      <c r="J17">
         <v>176</v>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>físico</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="M17" t="inlineStr">
         <is>
           <t>Ficção</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="N17" t="inlineStr">
         <is>
           <t>Sigrid Nunez</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>feminino</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>amarela</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>Estados Unidos</t>
-        </is>
-      </c>
       <c r="O17" t="inlineStr">
         <is>
           <t>TAG; TAG Curadoria</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/ZtwjtGrVpv5IA_PqzRdw1UzVFjU=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/122364329/OS_VULNERAVEIS_1716228229122364329SK-V11716228230B.jpg</t>
+        </is>
+      </c>
+      <c r="Q17">
+        <v>3.3</v>
+      </c>
+      <c r="R17">
+        <v>295</v>
+      </c>
+      <c r="S17" s="2">
+        <v>45503</v>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>https://www.skoob.com.br/os-vulneraveis-122364329ed122457493.html</t>
         </is>
       </c>
     </row>
@@ -1739,61 +1806,73 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="F18">
+        <v>17</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>A biblioteca da meia-noite</t>
         </is>
       </c>
-      <c r="E18">
+      <c r="H18">
         <v>2020</v>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>Bertrand Brasil</t>
         </is>
       </c>
-      <c r="G18">
+      <c r="J18">
         <v>320</v>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>físico</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="M18" t="inlineStr">
         <is>
           <t>Ficção científica</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="N18" t="inlineStr">
         <is>
           <t>Matt Haig</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>Estados Unidos</t>
-        </is>
-      </c>
       <c r="O18" t="inlineStr">
         <is>
           <t>TAG; TAG Inéditos</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr">
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/ISAyqpWG3q3D37qq9mZheUaMqVY=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/11927296/A_BIBLIOTECA_DA_MEIANOITE_162557999211927296SK-V11625579994B.jpg</t>
+        </is>
+      </c>
+      <c r="Q18">
+        <v>4.2</v>
+      </c>
+      <c r="R18">
+        <v>96945</v>
+      </c>
+      <c r="S18" s="2">
+        <v>45503</v>
+      </c>
+      <c r="T18" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/a-biblioteca-da-meia-noite-11927296ed11922234.html</t>
         </is>
@@ -1813,61 +1892,73 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="F19">
+        <v>18</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>Lua de Sangue</t>
         </is>
       </c>
-      <c r="E19">
+      <c r="H19">
         <v>2022</v>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>Record</t>
         </is>
       </c>
-      <c r="G19">
+      <c r="J19">
         <v>496</v>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="L19" t="inlineStr">
         <is>
           <t>físico</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="M19" t="inlineStr">
         <is>
           <t>Thriller; Mistério; Suspense</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="N19" t="inlineStr">
         <is>
           <t>Jo Nesbo</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>branca</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>Noruega</t>
-        </is>
-      </c>
       <c r="O19" t="inlineStr">
         <is>
           <t>TAG; TAG Inéditos</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/uQmZw_KpeCaWquJWFj0eR9bn9v4=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/122416209/LUA_DE_SANGUE_1723059350122416209SK-V11723059351B.jpg</t>
+        </is>
+      </c>
+      <c r="Q19">
+        <v>4.3</v>
+      </c>
+      <c r="R19">
+        <v>152</v>
+      </c>
+      <c r="S19" s="2">
+        <v>45503</v>
+      </c>
+      <c r="T19" t="inlineStr">
         <is>
           <t>https://www.skoob.com.br/lua-de-sangue-122416209ed122469308.html</t>
         </is>
@@ -1882,63 +1973,779 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>completo</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="F20">
+        <v>19</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Suicidas</t>
+        </is>
+      </c>
+      <c r="H20">
+        <v>2012</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Companhia das Letras</t>
+        </is>
+      </c>
+      <c r="J20">
+        <v>432</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>português</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>físico</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Thriller; Mistério; Suspense</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Raphael Montes</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Biblioteca SESC</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/ZQGeQnHV33qx7ruEmRM62Wy324k=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/253528/SUICIDAS_1498927512253528SK1498927512B.jpg</t>
+        </is>
+      </c>
+      <c r="Q20">
+        <v>4.5</v>
+      </c>
+      <c r="R20">
+        <v>42876</v>
+      </c>
+      <c r="S20" s="2">
+        <v>45503</v>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>https://www.skoob.com.br/suicidas-253528ed690354.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>2024</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>completo</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Maus</t>
+        </is>
+      </c>
+      <c r="H21">
+        <v>1991</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Companhia das Letras</t>
+        </is>
+      </c>
+      <c r="J21">
+        <v>296</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>português</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>físico</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Quadrinhos</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Art Spiegelman</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Biblioteca SESC</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/qc0O7yn02KZypDpOHlpGkND1iho=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/2259/MAUS_1299758721B.jpg</t>
+        </is>
+      </c>
+      <c r="Q21">
+        <v>4.7</v>
+      </c>
+      <c r="R21">
+        <v>33763</v>
+      </c>
+      <c r="S21" s="2">
+        <v>45503</v>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>https://www.skoob.com.br/maus-2259ed2994.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>2024</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>completo</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="F22">
+        <v>21</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>A fascinante história da matemática</t>
+        </is>
+      </c>
+      <c r="H22">
+        <v>2016</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Difel</t>
+        </is>
+      </c>
+      <c r="J22">
+        <v>264</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>português</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>ebook</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Divulgação científica</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Mickaël Launay</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/eYeZtdAtGf0zvW25QHlTH3yOxEk=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/918342/A_FASCINANTE_HISTORIA_DA_MATEM_1571241226918342SK1571241227B.jpg</t>
+        </is>
+      </c>
+      <c r="Q22">
+        <v>4.4</v>
+      </c>
+      <c r="R22">
+        <v>104</v>
+      </c>
+      <c r="S22" s="2">
+        <v>45512</v>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>https://www.skoob.com.br/a-fascinante-historia-da-matematica-918342ed924815.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>2024</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>completo</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="F23">
+        <v>22</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Jantar Secreto</t>
+        </is>
+      </c>
+      <c r="H23">
+        <v>2016</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Companhia das Letras</t>
+        </is>
+      </c>
+      <c r="J23">
+        <v>362</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>português</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>físico</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Thriller; Mistério; Suspense</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Raphael Montes</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Biblioteca SESC</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/2IFuMEEWqgjHw99Jxp2nwoXmkfc=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/619544/JANTAR_SECRETO_1476738260619544SK1476738260B.jpg</t>
+        </is>
+      </c>
+      <c r="Q23">
+        <v>4.4</v>
+      </c>
+      <c r="R23">
+        <v>54769</v>
+      </c>
+      <c r="S23" s="2">
+        <v>45503</v>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>https://www.skoob.com.br/jantar-secreto-619544ed620198.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>2024</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>completo</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="F24">
+        <v>23</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Uma mulher no escuro</t>
+        </is>
+      </c>
+      <c r="H24">
+        <v>2019</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Companhia das Letras</t>
+        </is>
+      </c>
+      <c r="J24">
+        <v>256</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>português</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>físico</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Thriller; Mistério; Suspense</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Raphael Montes</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Biblioteca SESC</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/sOVbMsu8801IpLZ2EinJdyyZ-84=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/868181/UMA_MULHER_NO_ESCURO_1555301729868181SK1555301729B.jpg</t>
+        </is>
+      </c>
+      <c r="Q24">
+        <v>4.2</v>
+      </c>
+      <c r="R24">
+        <v>26925</v>
+      </c>
+      <c r="S24" s="2">
+        <v>45512</v>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>https://www.skoob.com.br/uma-mulher-no-escuro-868181ed873853.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>2024</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>completo</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="F25">
+        <v>24</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Kindred: laços de sangue</t>
+        </is>
+      </c>
+      <c r="H25">
+        <v>1979</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Morro Branco</t>
+        </is>
+      </c>
+      <c r="J25">
+        <v>432</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>português</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>físico</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Ficção científica</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Octavia E. Butler</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Biblioteca SESC</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/VToOa8SjgUrRu-i4bAnhdiWIguA=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/686336/KINDRED_1505228890686336SK1505228891B.jpg</t>
+        </is>
+      </c>
+      <c r="Q25">
+        <v>4.5</v>
+      </c>
+      <c r="R25">
+        <v>12243</v>
+      </c>
+      <c r="S25" s="2">
+        <v>45512</v>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>https://www.skoob.com.br/kindred-686336ed688900.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>2024</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>completo</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="F26">
+        <v>25</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Alerta Vermelho</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Aleph</t>
+        </is>
+      </c>
+      <c r="J26">
+        <v>216</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>português</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>físico</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Ficção científica</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Martha Wells</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/n8G2e-ms-FHc5lygALvrgqz9w-k=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/122426363/ALERTA_VERMELHO_1714169701122426363SK-V11714169702B.jpg</t>
+        </is>
+      </c>
+      <c r="Q26">
+        <v>4.1</v>
+      </c>
+      <c r="R26">
+        <v>249</v>
+      </c>
+      <c r="S26" s="2">
+        <v>45512</v>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>https://www.skoob.com.br/alerta-vermelho-122426363ed122429742.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>2024</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>lendo</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Suicidas</t>
-        </is>
-      </c>
-      <c r="E20">
-        <v>2012</v>
-      </c>
-      <c r="F20" t="inlineStr">
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Uma família feliz</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
         <is>
           <t>Companhia das Letras</t>
         </is>
       </c>
-      <c r="G20">
-        <v>432</v>
-      </c>
-      <c r="H20" t="inlineStr">
+      <c r="K27" t="inlineStr">
         <is>
           <t>português</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="L27" t="inlineStr">
         <is>
           <t>físico</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="M27" t="inlineStr">
         <is>
           <t>Thriller; Mistério; Suspense</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="N27" t="inlineStr">
         <is>
           <t>Raphael Montes</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>masculino</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>Biblioteca SESC</t>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Biblioteca Parque Villa-Lobos</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/bxRtc0Ox-u-SHJ_j6woiQWbktc0=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/122414997/UMA_FAMILIA_FELIZ_1706015871122414997SK-V11706015872B.jpg</t>
+        </is>
+      </c>
+      <c r="Q27">
+        <v>4.1</v>
+      </c>
+      <c r="R27">
+        <v>12306</v>
+      </c>
+      <c r="S27" s="2">
+        <v>45512</v>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>https://www.skoob.com.br/uma-familia-feliz-122414997ed122417542.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>2024</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>lendo</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Coração de Aço (Os Executores #1)</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Aleph</t>
+        </is>
+      </c>
+      <c r="J28">
+        <v>376</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>português</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>ebook</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Brandon Sanderson</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>https://img.skoob.com.br/PtBOCkaPld5fjodskvl_7amI2nk=/200x/center/top/smart/filters:format(jpeg)/https://skoob.s3.amazonaws.com/livros/615632/CORACAO_DE_ACO_1518718820615632SK1518718821B.jpg</t>
+        </is>
+      </c>
+      <c r="Q28">
+        <v>4.3</v>
+      </c>
+      <c r="R28">
+        <v>3631</v>
+      </c>
+      <c r="S28" s="2">
+        <v>45512</v>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>https://www.skoob.com.br/coracao-de-aco-615632ed616214.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>2024</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>lendo</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Assistente do Vilão</t>
+        </is>
+      </c>
+      <c r="H29">
+        <v>2023</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Alt</t>
+        </is>
+      </c>
+      <c r="J29">
+        <v>512</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>português</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>ebook</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Fantasia</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Hannah Nicole Maehrer</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Skeelo</t>
         </is>
       </c>
     </row>

</xml_diff>